<commit_message>
added conversion factors for Flows and some missing Other
</commit_message>
<xml_diff>
--- a/dev/energyscope_data/CH/unit_conversion_3.10.1.xlsx
+++ b/dev/energyscope_data/CH/unit_conversion_3.10.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\mescal\dev\energyscope_data\CH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659BAC18-47AB-46EA-9F46-5F08CF0CAB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD36CC35-C890-431F-BB40-3DBE4B5F2E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2454" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2695" uniqueCount="512">
   <si>
     <t>Name</t>
   </si>
@@ -1527,6 +1527,48 @@
   </si>
   <si>
     <t>density of syngas: (0.470 kg/m3): \cite{vandergiesen2014}</t>
+  </si>
+  <si>
+    <t>Flow</t>
+  </si>
+  <si>
+    <t>BIO_DIESEL</t>
+  </si>
+  <si>
+    <t>CO2_C</t>
+  </si>
+  <si>
+    <t>ELECTRICITY_HV</t>
+  </si>
+  <si>
+    <t>ELECTRICITY_LV</t>
+  </si>
+  <si>
+    <t>ELECTRICITY_MV</t>
+  </si>
+  <si>
+    <t>HEAT_HIGH_T</t>
+  </si>
+  <si>
+    <t>HEAT_LOW_T_DECEN</t>
+  </si>
+  <si>
+    <t>HEAT_LOW_T_DHN</t>
+  </si>
+  <si>
+    <t>benzene</t>
+  </si>
+  <si>
+    <t>propylene</t>
+  </si>
+  <si>
+    <t>methanol</t>
+  </si>
+  <si>
+    <t>ethylene</t>
+  </si>
+  <si>
+    <t>Biogas LHV (22.73 MJ/m3): \cite{wernet2016}</t>
   </si>
 </sst>
 </file>
@@ -1585,11 +1627,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1894,10 +1937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F516"/>
+  <dimension ref="A1:F567"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A514" workbookViewId="0">
+      <selection activeCell="C521" sqref="C521"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12253,6 +12296,985 @@
         <v>487</v>
       </c>
     </row>
+    <row r="517" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A517" t="s">
+        <v>507</v>
+      </c>
+      <c r="B517" t="s">
+        <v>350</v>
+      </c>
+      <c r="C517">
+        <v>8.4705881999999996E-2</v>
+      </c>
+      <c r="D517" t="s">
+        <v>351</v>
+      </c>
+      <c r="E517" t="s">
+        <v>356</v>
+      </c>
+      <c r="F517" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="518" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A518" t="s">
+        <v>508</v>
+      </c>
+      <c r="B518" t="s">
+        <v>350</v>
+      </c>
+      <c r="C518">
+        <v>7.8604335999999997E-2</v>
+      </c>
+      <c r="D518" t="s">
+        <v>351</v>
+      </c>
+      <c r="E518" t="s">
+        <v>356</v>
+      </c>
+      <c r="F518" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="519" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A519" t="s">
+        <v>509</v>
+      </c>
+      <c r="B519" t="s">
+        <v>350</v>
+      </c>
+      <c r="C519">
+        <v>0.180505415</v>
+      </c>
+      <c r="D519" t="s">
+        <v>351</v>
+      </c>
+      <c r="E519" t="s">
+        <v>356</v>
+      </c>
+      <c r="F519" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="520" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A520" t="s">
+        <v>510</v>
+      </c>
+      <c r="B520" t="s">
+        <v>350</v>
+      </c>
+      <c r="C520">
+        <v>7.1591926E-2</v>
+      </c>
+      <c r="D520" t="s">
+        <v>351</v>
+      </c>
+      <c r="E520" t="s">
+        <v>356</v>
+      </c>
+      <c r="F520" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="521" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A521" t="s">
+        <v>328</v>
+      </c>
+      <c r="B521" t="s">
+        <v>350</v>
+      </c>
+      <c r="C521">
+        <f>3.6/22.73</f>
+        <v>0.1583809942806863</v>
+      </c>
+      <c r="D521" t="s">
+        <v>353</v>
+      </c>
+      <c r="E521" t="s">
+        <v>356</v>
+      </c>
+      <c r="F521" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="522" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A522" t="s">
+        <v>6</v>
+      </c>
+      <c r="B522" t="s">
+        <v>498</v>
+      </c>
+      <c r="C522">
+        <v>0.24742268000000001</v>
+      </c>
+      <c r="D522" t="s">
+        <v>351</v>
+      </c>
+      <c r="E522" t="s">
+        <v>356</v>
+      </c>
+      <c r="F522" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="523" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A523" t="s">
+        <v>7</v>
+      </c>
+      <c r="B523" t="s">
+        <v>498</v>
+      </c>
+      <c r="C523">
+        <v>0.121654501</v>
+      </c>
+      <c r="D523" t="s">
+        <v>351</v>
+      </c>
+      <c r="E523" t="s">
+        <v>356</v>
+      </c>
+      <c r="F523" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="524" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A524" t="s">
+        <v>20</v>
+      </c>
+      <c r="B524" t="s">
+        <v>498</v>
+      </c>
+      <c r="C524">
+        <v>8.4705881999999996E-2</v>
+      </c>
+      <c r="D524" t="s">
+        <v>351</v>
+      </c>
+      <c r="E524" t="s">
+        <v>356</v>
+      </c>
+      <c r="F524" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="525" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A525" t="s">
+        <v>499</v>
+      </c>
+      <c r="B525" t="s">
+        <v>498</v>
+      </c>
+      <c r="C525">
+        <v>8.4530854000000002E-2</v>
+      </c>
+      <c r="D525" t="s">
+        <v>351</v>
+      </c>
+      <c r="E525" t="s">
+        <v>356</v>
+      </c>
+      <c r="F525" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="526" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A526" t="s">
+        <v>500</v>
+      </c>
+      <c r="B526" t="s">
+        <v>498</v>
+      </c>
+      <c r="C526">
+        <v>1</v>
+      </c>
+      <c r="D526" t="s">
+        <v>351</v>
+      </c>
+      <c r="E526" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="527" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A527" t="s">
+        <v>67</v>
+      </c>
+      <c r="B527" t="s">
+        <v>498</v>
+      </c>
+      <c r="C527">
+        <v>0.128986027</v>
+      </c>
+      <c r="D527" t="s">
+        <v>351</v>
+      </c>
+      <c r="E527" t="s">
+        <v>356</v>
+      </c>
+      <c r="F527" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="528" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A528" t="s">
+        <v>132</v>
+      </c>
+      <c r="B528" t="s">
+        <v>498</v>
+      </c>
+      <c r="C528">
+        <v>8.4530854000000002E-2</v>
+      </c>
+      <c r="D528" t="s">
+        <v>351</v>
+      </c>
+      <c r="E528" t="s">
+        <v>356</v>
+      </c>
+      <c r="F528" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="529" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A529" t="s">
+        <v>139</v>
+      </c>
+      <c r="B529" t="s">
+        <v>498</v>
+      </c>
+      <c r="C529">
+        <v>1</v>
+      </c>
+      <c r="D529" t="s">
+        <v>356</v>
+      </c>
+      <c r="E529" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="530" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A530" t="s">
+        <v>501</v>
+      </c>
+      <c r="B530" t="s">
+        <v>498</v>
+      </c>
+      <c r="C530">
+        <v>1</v>
+      </c>
+      <c r="D530" t="s">
+        <v>356</v>
+      </c>
+      <c r="E530" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="531" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A531" t="s">
+        <v>502</v>
+      </c>
+      <c r="B531" t="s">
+        <v>498</v>
+      </c>
+      <c r="C531">
+        <v>1</v>
+      </c>
+      <c r="D531" t="s">
+        <v>356</v>
+      </c>
+      <c r="E531" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="532" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A532" t="s">
+        <v>503</v>
+      </c>
+      <c r="B532" t="s">
+        <v>498</v>
+      </c>
+      <c r="C532">
+        <v>1</v>
+      </c>
+      <c r="D532" t="s">
+        <v>356</v>
+      </c>
+      <c r="E532" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="533" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A533" t="s">
+        <v>143</v>
+      </c>
+      <c r="B533" t="s">
+        <v>498</v>
+      </c>
+      <c r="C533">
+        <v>7.5301204999999996E-2</v>
+      </c>
+      <c r="D533" t="s">
+        <v>351</v>
+      </c>
+      <c r="E533" t="s">
+        <v>356</v>
+      </c>
+      <c r="F533" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="534" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A534" t="s">
+        <v>147</v>
+      </c>
+      <c r="B534" t="s">
+        <v>498</v>
+      </c>
+      <c r="C534">
+        <v>0.11399620000000001</v>
+      </c>
+      <c r="D534" t="s">
+        <v>351</v>
+      </c>
+      <c r="E534" t="s">
+        <v>356</v>
+      </c>
+      <c r="F534" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="535" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A535" t="s">
+        <v>149</v>
+      </c>
+      <c r="B535" t="s">
+        <v>498</v>
+      </c>
+      <c r="C535">
+        <v>8.7937856999999994E-2</v>
+      </c>
+      <c r="D535" t="s">
+        <v>351</v>
+      </c>
+      <c r="E535" t="s">
+        <v>356</v>
+      </c>
+      <c r="F535" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="536" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A536" t="s">
+        <v>150</v>
+      </c>
+      <c r="B536" t="s">
+        <v>498</v>
+      </c>
+      <c r="C536">
+        <v>7.1591926E-2</v>
+      </c>
+      <c r="D536" t="s">
+        <v>351</v>
+      </c>
+      <c r="E536" t="s">
+        <v>356</v>
+      </c>
+      <c r="F536" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="537" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A537" t="s">
+        <v>162</v>
+      </c>
+      <c r="B537" t="s">
+        <v>498</v>
+      </c>
+      <c r="C537">
+        <v>8.4705881999999996E-2</v>
+      </c>
+      <c r="D537" t="s">
+        <v>351</v>
+      </c>
+      <c r="E537" t="s">
+        <v>356</v>
+      </c>
+      <c r="F537" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="538" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A538" t="s">
+        <v>168</v>
+      </c>
+      <c r="B538" t="s">
+        <v>498</v>
+      </c>
+      <c r="C538">
+        <v>3.0030029999999999E-2</v>
+      </c>
+      <c r="D538" t="s">
+        <v>351</v>
+      </c>
+      <c r="E538" t="s">
+        <v>356</v>
+      </c>
+      <c r="F538" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="539" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A539" t="s">
+        <v>175</v>
+      </c>
+      <c r="B539" t="s">
+        <v>498</v>
+      </c>
+      <c r="C539">
+        <v>3.0030029999999999E-2</v>
+      </c>
+      <c r="D539" t="s">
+        <v>351</v>
+      </c>
+      <c r="E539" t="s">
+        <v>356</v>
+      </c>
+      <c r="F539" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="540" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A540" t="s">
+        <v>176</v>
+      </c>
+      <c r="B540" t="s">
+        <v>498</v>
+      </c>
+      <c r="C540">
+        <v>3.0030029999999999E-2</v>
+      </c>
+      <c r="D540" t="s">
+        <v>351</v>
+      </c>
+      <c r="E540" t="s">
+        <v>356</v>
+      </c>
+      <c r="F540" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="541" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A541" t="s">
+        <v>177</v>
+      </c>
+      <c r="B541" t="s">
+        <v>498</v>
+      </c>
+      <c r="C541">
+        <v>3.0030029999999999E-2</v>
+      </c>
+      <c r="D541" t="s">
+        <v>351</v>
+      </c>
+      <c r="E541" t="s">
+        <v>356</v>
+      </c>
+      <c r="F541" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="542" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A542" t="s">
+        <v>504</v>
+      </c>
+      <c r="B542" t="s">
+        <v>498</v>
+      </c>
+      <c r="C542">
+        <v>3.6</v>
+      </c>
+      <c r="D542" t="s">
+        <v>357</v>
+      </c>
+      <c r="E542" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="543" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A543" t="s">
+        <v>505</v>
+      </c>
+      <c r="B543" t="s">
+        <v>498</v>
+      </c>
+      <c r="C543">
+        <v>3.6</v>
+      </c>
+      <c r="D543" t="s">
+        <v>357</v>
+      </c>
+      <c r="E543" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="544" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A544" t="s">
+        <v>506</v>
+      </c>
+      <c r="B544" t="s">
+        <v>498</v>
+      </c>
+      <c r="C544">
+        <v>3.6</v>
+      </c>
+      <c r="D544" t="s">
+        <v>357</v>
+      </c>
+      <c r="E544" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="545" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A545" t="s">
+        <v>213</v>
+      </c>
+      <c r="B545" t="s">
+        <v>498</v>
+      </c>
+      <c r="C545">
+        <v>8.3720929999999999E-2</v>
+      </c>
+      <c r="D545" t="s">
+        <v>351</v>
+      </c>
+      <c r="E545" t="s">
+        <v>356</v>
+      </c>
+      <c r="F545" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="546" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A546" t="s">
+        <v>214</v>
+      </c>
+      <c r="B546" t="s">
+        <v>498</v>
+      </c>
+      <c r="C546">
+        <v>8.4507042000000004E-2</v>
+      </c>
+      <c r="D546" t="s">
+        <v>351</v>
+      </c>
+      <c r="E546" t="s">
+        <v>356</v>
+      </c>
+      <c r="F546" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="547" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A547" t="s">
+        <v>215</v>
+      </c>
+      <c r="B547" t="s">
+        <v>498</v>
+      </c>
+      <c r="C547">
+        <v>9.2307691999999997E-2</v>
+      </c>
+      <c r="D547" t="s">
+        <v>353</v>
+      </c>
+      <c r="E547" t="s">
+        <v>356</v>
+      </c>
+      <c r="F547" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="548" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A548" t="s">
+        <v>222</v>
+      </c>
+      <c r="B548" t="s">
+        <v>498</v>
+      </c>
+      <c r="C548">
+        <v>0.180505415</v>
+      </c>
+      <c r="D548" t="s">
+        <v>351</v>
+      </c>
+      <c r="E548" t="s">
+        <v>356</v>
+      </c>
+      <c r="F548" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="549" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A549" t="s">
+        <v>236</v>
+      </c>
+      <c r="B549" t="s">
+        <v>498</v>
+      </c>
+      <c r="C549">
+        <v>9.2307691999999997E-2</v>
+      </c>
+      <c r="D549" t="s">
+        <v>353</v>
+      </c>
+      <c r="E549" t="s">
+        <v>356</v>
+      </c>
+      <c r="F549" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="550" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A550" t="s">
+        <v>243</v>
+      </c>
+      <c r="B550" t="s">
+        <v>498</v>
+      </c>
+      <c r="C550">
+        <v>9.8244372999999996E-2</v>
+      </c>
+      <c r="D550" t="s">
+        <v>353</v>
+      </c>
+      <c r="E550" t="s">
+        <v>356</v>
+      </c>
+      <c r="F550" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="551" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A551" t="s">
+        <v>244</v>
+      </c>
+      <c r="B551" t="s">
+        <v>498</v>
+      </c>
+      <c r="C551">
+        <v>9.8244372999999996E-2</v>
+      </c>
+      <c r="D551" t="s">
+        <v>353</v>
+      </c>
+      <c r="E551" t="s">
+        <v>356</v>
+      </c>
+      <c r="F551" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="552" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A552" t="s">
+        <v>245</v>
+      </c>
+      <c r="B552" t="s">
+        <v>498</v>
+      </c>
+      <c r="C552">
+        <v>7.7419354999999995E-2</v>
+      </c>
+      <c r="D552" t="s">
+        <v>351</v>
+      </c>
+      <c r="E552" t="s">
+        <v>356</v>
+      </c>
+      <c r="F552" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="553" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A553" t="s">
+        <v>254</v>
+      </c>
+      <c r="B553" t="s">
+        <v>498</v>
+      </c>
+      <c r="C553">
+        <v>1</v>
+      </c>
+      <c r="D553" t="s">
+        <v>351</v>
+      </c>
+      <c r="E553" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="554" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A554" t="s">
+        <v>260</v>
+      </c>
+      <c r="B554" t="s">
+        <v>498</v>
+      </c>
+      <c r="C554">
+        <v>1</v>
+      </c>
+      <c r="D554" t="s">
+        <v>351</v>
+      </c>
+      <c r="E554" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="555" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A555" t="s">
+        <v>262</v>
+      </c>
+      <c r="B555" t="s">
+        <v>498</v>
+      </c>
+      <c r="C555">
+        <v>0.110939908</v>
+      </c>
+      <c r="D555" t="s">
+        <v>351</v>
+      </c>
+      <c r="E555" t="s">
+        <v>356</v>
+      </c>
+      <c r="F555" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="556" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A556" t="s">
+        <v>265</v>
+      </c>
+      <c r="B556" t="s">
+        <v>498</v>
+      </c>
+      <c r="C556">
+        <v>1</v>
+      </c>
+      <c r="D556" t="s">
+        <v>351</v>
+      </c>
+      <c r="E556" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="557" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A557" t="s">
+        <v>266</v>
+      </c>
+      <c r="B557" t="s">
+        <v>498</v>
+      </c>
+      <c r="C557">
+        <v>7.8604335999999997E-2</v>
+      </c>
+      <c r="D557" t="s">
+        <v>351</v>
+      </c>
+      <c r="E557" t="s">
+        <v>356</v>
+      </c>
+      <c r="F557" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="558" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A558" t="s">
+        <v>267</v>
+      </c>
+      <c r="B558" t="s">
+        <v>498</v>
+      </c>
+      <c r="C558">
+        <v>1</v>
+      </c>
+      <c r="D558" t="s">
+        <v>351</v>
+      </c>
+      <c r="E558" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="559" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A559" t="s">
+        <v>269</v>
+      </c>
+      <c r="B559" t="s">
+        <v>498</v>
+      </c>
+      <c r="C559">
+        <v>1</v>
+      </c>
+      <c r="D559" t="s">
+        <v>351</v>
+      </c>
+      <c r="E559" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="560" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A560" t="s">
+        <v>277</v>
+      </c>
+      <c r="B560" t="s">
+        <v>498</v>
+      </c>
+      <c r="C560">
+        <v>9.8244372999999996E-2</v>
+      </c>
+      <c r="D560" t="s">
+        <v>353</v>
+      </c>
+      <c r="E560" t="s">
+        <v>356</v>
+      </c>
+      <c r="F560" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="561" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A561" t="s">
+        <v>287</v>
+      </c>
+      <c r="B561" t="s">
+        <v>498</v>
+      </c>
+      <c r="C561">
+        <v>1</v>
+      </c>
+      <c r="D561" t="s">
+        <v>351</v>
+      </c>
+      <c r="E561" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="562" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A562" t="s">
+        <v>289</v>
+      </c>
+      <c r="B562" t="s">
+        <v>498</v>
+      </c>
+      <c r="C562">
+        <v>8.4845628000000006E-2</v>
+      </c>
+      <c r="D562" t="s">
+        <v>351</v>
+      </c>
+      <c r="E562" t="s">
+        <v>356</v>
+      </c>
+      <c r="F562" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="563" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A563" t="s">
+        <v>319</v>
+      </c>
+      <c r="B563" t="s">
+        <v>498</v>
+      </c>
+      <c r="C563" s="2">
+        <v>9.23077E-7</v>
+      </c>
+      <c r="D563" t="s">
+        <v>351</v>
+      </c>
+      <c r="E563" t="s">
+        <v>356</v>
+      </c>
+      <c r="F563" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="564" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A564" t="s">
+        <v>320</v>
+      </c>
+      <c r="B564" t="s">
+        <v>498</v>
+      </c>
+      <c r="C564">
+        <v>-0.29149797599999999</v>
+      </c>
+      <c r="D564" t="s">
+        <v>351</v>
+      </c>
+      <c r="E564" t="s">
+        <v>356</v>
+      </c>
+      <c r="F564" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="565" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A565" t="s">
+        <v>323</v>
+      </c>
+      <c r="B565" t="s">
+        <v>498</v>
+      </c>
+      <c r="C565">
+        <v>0.43483512499999999</v>
+      </c>
+      <c r="D565" t="s">
+        <v>351</v>
+      </c>
+      <c r="E565" t="s">
+        <v>356</v>
+      </c>
+      <c r="F565" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="566" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A566" t="s">
+        <v>325</v>
+      </c>
+      <c r="B566" t="s">
+        <v>498</v>
+      </c>
+      <c r="C566">
+        <v>0.23376623399999999</v>
+      </c>
+      <c r="D566" t="s">
+        <v>351</v>
+      </c>
+      <c r="E566" t="s">
+        <v>356</v>
+      </c>
+      <c r="F566" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="567" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A567" t="s">
+        <v>327</v>
+      </c>
+      <c r="B567" t="s">
+        <v>498</v>
+      </c>
+      <c r="C567">
+        <v>8.7888479000000005E-2</v>
+      </c>
+      <c r="D567" t="s">
+        <v>351</v>
+      </c>
+      <c r="E567" t="s">
+        <v>356</v>
+      </c>
+      <c r="F567" t="s">
+        <v>485</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>